<commit_message>
Restructure ontology: remove mfd_hab1=Urban if mfd_areatype=Urban
</commit_message>
<xml_diff>
--- a/analysis/metadata/P02_1/P02_1_minimal_metadata.xlsx
+++ b/analysis/metadata/P02_1/P02_1_minimal_metadata.xlsx
@@ -687,7 +687,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -726,11 +726,6 @@
         </is>
       </c>
       <c r="N5" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -1495,7 +1490,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1534,11 +1529,6 @@
         </is>
       </c>
       <c r="N16" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O16" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -1641,7 +1631,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1680,11 +1670,6 @@
         </is>
       </c>
       <c r="N18" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -1792,7 +1777,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1831,11 +1816,6 @@
         </is>
       </c>
       <c r="N20" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O20" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -2172,7 +2152,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -2211,11 +2191,6 @@
         </is>
       </c>
       <c r="N25" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -2620,7 +2595,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2659,11 +2634,6 @@
         </is>
       </c>
       <c r="N31" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O31" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -3380,7 +3350,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -3419,11 +3389,6 @@
         </is>
       </c>
       <c r="N41" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -3901,7 +3866,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -3940,11 +3905,6 @@
         </is>
       </c>
       <c r="N48" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O48" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -4792,7 +4752,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -4831,11 +4791,6 @@
         </is>
       </c>
       <c r="N60" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O60" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>
@@ -5298,7 +5253,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>6100</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -5337,11 +5292,6 @@
         </is>
       </c>
       <c r="N67" t="inlineStr">
-        <is>
-          <t>Urban</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr">
         <is>
           <t>Roadside</t>
         </is>

</xml_diff>